<commit_message>
Improved Feature Import Kelas Mapel
</commit_message>
<xml_diff>
--- a/public/excel/template-kelas-mapel.xlsx
+++ b/public/excel/template-kelas-mapel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ketuntasan\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFACA22-1D0E-44B8-BF16-7108115A27BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5BF749-64FC-4A3E-A82E-C7CB12DDD8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15AB2BBF-ED13-4B5E-B4AF-6647F79E46D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{15AB2BBF-ED13-4B5E-B4AF-6647F79E46D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <r>
       <rPr>
@@ -87,56 +84,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PETUNJUK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SILAHKAN MASUKKAN KODE MAPEL
-DI DALAM SYMBOL [ ]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PETUNJUK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SILAHKAN MASUKKAN KODE GURU
-DI DALAM SYMBOL [ ]</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">MASUKKAN 
 </t>
     </r>
@@ -170,6 +117,12 @@
     </r>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">MASUKKAN
 </t>
@@ -183,37 +136,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>KODE MAPEL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">MASUKKAN
-</t>
-    </r>
+      <t>KODE GURU MAPEL</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PETUNJUK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>KODE GURU</t>
-    </r>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>[1]</t>
-  </si>
-  <si>
-    <t>[2]</t>
-  </si>
-  <si>
-    <t>[3]</t>
+      <t xml:space="preserve">
+SILAHKAN MASUKKAN KODE GURU MAPEL
+DI DALAM SYMBOL [ ]</t>
+    </r>
+  </si>
+  <si>
+    <t>[2,1]</t>
+  </si>
+  <si>
+    <t>[2,2]</t>
   </si>
 </sst>
 </file>
@@ -602,20 +557,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1862F56C-2033-4F79-95FA-E6BE6F9DAD95}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="26.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -623,38 +578,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>